<commit_message>
- Fixed length of Picoblade cable on solenoid driver BOM. - Small changes to breakout board enclosure readme.
</commit_message>
<xml_diff>
--- a/Nine_poke/solenoid_driver_1_0/solenoid_driver_BOM.xlsx
+++ b/Nine_poke/solenoid_driver_1_0/solenoid_driver_BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Hardware development\Eagle projects\Pokes\nine_poke\solenoid_driver_1_0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Hardware development\pyControl_hardware\Nine_poke\solenoid_driver_1_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="41">
   <si>
     <t>IC1</t>
   </si>
@@ -137,10 +137,16 @@
     <t>Molex</t>
   </si>
   <si>
-    <t>Picoblade cable - 5 way 100mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15134-0501 </t>
+    <t>Picoblade cable - 5 way 50mm</t>
+  </si>
+  <si>
+    <t>15134-0500</t>
+  </si>
+  <si>
+    <t>OC_RS</t>
+  </si>
+  <si>
+    <t>125-0735</t>
   </si>
 </sst>
 </file>
@@ -459,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="A14" sqref="A14:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,7 +479,7 @@
     <col min="7" max="7" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -498,8 +504,11 @@
       <c r="H1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -525,7 +534,7 @@
         <v>1332086</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -548,7 +557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -574,7 +583,7 @@
         <v>1125360</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -600,7 +609,7 @@
         <v>1803308</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -626,7 +635,7 @@
         <v>1803308</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -652,7 +661,7 @@
         <v>1803308</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -678,7 +687,7 @@
         <v>1803308</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -704,7 +713,7 @@
         <v>1803308</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -730,7 +739,7 @@
         <v>1803308</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -756,7 +765,7 @@
         <v>1803308</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -782,7 +791,7 @@
         <v>1803308</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -803,6 +812,9 @@
       </c>
       <c r="G14" t="s">
         <v>38</v>
+      </c>
+      <c r="H14" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>